<commit_message>
Database integration functional, optimisation needed
</commit_message>
<xml_diff>
--- a/Database tables.xlsx
+++ b/Database tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl.sharepoint.com/teams/S6projects22-23-Insyte/Gedeelde documenten/Insyte/ESE/Software/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="8_{C4C697FA-65F9-470A-84F0-E6A8707095AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{465BBDDD-DECD-4B8C-85B6-F7950F3EBE4D}"/>
+  <xr:revisionPtr revIDLastSave="291" documentId="8_{C4C697FA-65F9-470A-84F0-E6A8707095AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF9FC86A-0295-4800-A844-02BB2F76BCBD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{06156DA9-2425-482B-9CDE-F24571497A90}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{06156DA9-2425-482B-9CDE-F24571497A90}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>mac_adress</t>
   </si>
@@ -227,22 +227,7 @@
     <t>00:2B:44:11:3A:C</t>
   </si>
   <si>
-    <t>mqtt-topics</t>
-  </si>
-  <si>
-    <t>/data/sensors/temperature</t>
-  </si>
-  <si>
-    <t>/data/sensors/humidity</t>
-  </si>
-  <si>
-    <t>/data/sensors/lidposition</t>
-  </si>
-  <si>
     <t>housenr</t>
-  </si>
-  <si>
-    <t>topicidnr</t>
   </si>
   <si>
     <t>idnr</t>
@@ -670,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915CABEF-E1C4-4E4E-8558-142F6686C6E3}">
-  <dimension ref="B5:M41"/>
+  <dimension ref="B5:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,9 +670,11 @@
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="14.109375" customWidth="1"/>
     <col min="9" max="9" width="23.5546875" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
     <col min="11" max="11" width="11.88671875" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" customWidth="1"/>
     <col min="13" max="13" width="24.5546875" customWidth="1"/>
+    <col min="14" max="14" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
@@ -700,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -734,7 +721,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -743,13 +730,13 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
         <v>4</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
         <v>5</v>
@@ -782,10 +769,10 @@
       </c>
       <c r="I13" s="2"/>
       <c r="K13" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="L13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
@@ -881,7 +868,7 @@
       </c>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>5</v>
       </c>
@@ -908,17 +895,17 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>0</v>
       </c>
@@ -946,10 +933,10 @@
       <c r="K20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>35</v>
       </c>
@@ -968,17 +955,20 @@
       <c r="I21" s="2">
         <v>1</v>
       </c>
-      <c r="K21" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="K21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M21" t="s">
         <v>16</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>61</v>
       </c>
@@ -997,17 +987,20 @@
       <c r="I22" s="2">
         <v>2</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="2">
         <v>1</v>
       </c>
-      <c r="L22" s="2">
+      <c r="M22" s="2">
         <v>7</v>
       </c>
-      <c r="M22" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>62</v>
       </c>
@@ -1026,17 +1019,20 @@
       <c r="I23" s="2">
         <v>3</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" t="s">
+        <v>61</v>
+      </c>
+      <c r="L23" s="2">
         <v>2</v>
       </c>
-      <c r="L23" s="2">
+      <c r="M23" s="2">
         <v>90</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="N23" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>37</v>
       </c>
@@ -1055,17 +1051,20 @@
       <c r="I24" s="2">
         <v>2</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L24" s="2">
         <v>3</v>
       </c>
-      <c r="L24" s="2">
+      <c r="M24" s="2">
         <v>1</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="N24" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>38</v>
       </c>
@@ -1085,42 +1084,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="2">
-        <v>2</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="2">
-        <v>3</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="2">
-        <v>4</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>66</v>
-      </c>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" s="2"/>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40" s="2"/>
@@ -1135,4 +1116,271 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050EA777A35085441BA1BE2161358D91E" ma:contentTypeVersion="12" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="4c2f5df5c6316f1dea17ec6a614fca1f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e79b233-b289-407c-a2c1-6923f31521dd" xmlns:ns3="c621cafd-5eb4-468b-84e8-15f5c7a0b856" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="307d1b2198d7743b3bb3c97192c06102" ns2:_="" ns3:_="">
+    <xsd:import namespace="1e79b233-b289-407c-a2c1-6923f31521dd"/>
+    <xsd:import namespace="c621cafd-5eb4-468b-84e8-15f5c7a0b856"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1e79b233-b289-407c-a2c1-6923f31521dd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Gedeeld met" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Gedeeld met details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c621cafd-5eb4-468b-84e8-15f5c7a0b856" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Afbeeldingtags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="f6aa0a0a-ab1b-4084-9454-0fab04725976" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhoudstype"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c621cafd-5eb4-468b-84e8-15f5c7a0b856">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BE307DB-8C6A-41CD-9097-1DB3102D80C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54685ABA-E87D-4F07-8C51-0000AD5F8C44}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e79b233-b289-407c-a2c1-6923f31521dd"/>
+    <ds:schemaRef ds:uri="c621cafd-5eb4-468b-84e8-15f5c7a0b856"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1067267C-085B-4BFC-9D2F-D0D2D744F0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c621cafd-5eb4-468b-84e8-15f5c7a0b856"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
database structure completed for now. Database filled with data, no sensor data yet
</commit_message>
<xml_diff>
--- a/Database tables.xlsx
+++ b/Database tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl.sharepoint.com/teams/S6projects22-23-Insyte/Gedeelde documenten/Insyte/ESE/Software/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="291" documentId="8_{C4C697FA-65F9-470A-84F0-E6A8707095AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF9FC86A-0295-4800-A844-02BB2F76BCBD}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="8_{C4C697FA-65F9-470A-84F0-E6A8707095AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A583E52-BF0B-43D6-AA22-0B4AB0D4E9E1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{06156DA9-2425-482B-9CDE-F24571497A90}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{06156DA9-2425-482B-9CDE-F24571497A90}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
   <si>
     <t>mac_adress</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Koelaan</t>
   </si>
   <si>
-    <t>Eslweide</t>
-  </si>
-  <si>
     <t>Kortelaantje</t>
   </si>
   <si>
@@ -240,6 +237,21 @@
   </si>
   <si>
     <t>sensor_idnr</t>
+  </si>
+  <si>
+    <t>Elsweide</t>
+  </si>
+  <si>
+    <t>/data/sensors/</t>
+  </si>
+  <si>
+    <t>sensor_unit</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -658,7 +670,7 @@
   <dimension ref="B5:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,12 +699,12 @@
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -700,7 +712,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -708,7 +720,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -721,7 +733,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -730,13 +742,13 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
         <v>4</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H12" t="s">
         <v>5</v>
@@ -769,10 +781,13 @@
       </c>
       <c r="I13" s="2"/>
       <c r="K13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L13" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="M13" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
@@ -802,9 +817,11 @@
         <v>1</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M14" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
@@ -833,9 +850,11 @@
         <v>2</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M15" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
@@ -857,14 +876,14 @@
         <v>145</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="I16" s="2"/>
       <c r="K16" s="2">
         <v>3</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M16" s="2"/>
     </row>
@@ -888,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I17" s="2"/>
       <c r="K17" s="2"/>
@@ -938,28 +957,28 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H21" s="2">
         <v>1883</v>
       </c>
-      <c r="I21" s="2">
-        <v>1</v>
+      <c r="I21" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>0</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M21" t="s">
         <v>16</v>
@@ -970,25 +989,25 @@
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="2">
         <v>1883</v>
       </c>
-      <c r="I22" s="2">
-        <v>2</v>
+      <c r="I22" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="K22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L22" s="2">
         <v>1</v>
@@ -997,30 +1016,30 @@
         <v>7</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H23" s="2">
         <v>1883</v>
       </c>
-      <c r="I23" s="2">
-        <v>3</v>
+      <c r="I23" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="K23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L23" s="2">
         <v>2</v>
@@ -1029,30 +1048,30 @@
         <v>90</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H24" s="2">
         <v>1883</v>
       </c>
-      <c r="I24" s="2">
-        <v>2</v>
+      <c r="I24" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="K24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L24" s="2">
         <v>3</v>
@@ -1061,27 +1080,27 @@
         <v>1</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H25" s="2">
         <v>1883</v>
       </c>
-      <c r="I25" s="2">
-        <v>3</v>
+      <c r="I25" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">

</xml_diff>